<commit_message>
Preprocess added to treat instances of NO and NaN
</commit_message>
<xml_diff>
--- a/Data-Analysis/CategoricalStats.xlsx
+++ b/Data-Analysis/CategoricalStats.xlsx
@@ -71,9 +71,6 @@
     <t>vomitos</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>Persistente</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>prueba_torniquete</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>Negativa</t>
@@ -1344,7 +1344,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>241</v>
@@ -1381,57 +1381,40 @@
         <v>625</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>3670</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>745</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="E3">
-        <v>3670</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>745</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>180</v>
+        <v>103</v>
       </c>
       <c r="D4">
-        <v>382</v>
+        <v>35</v>
       </c>
       <c r="E4">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>103</v>
-      </c>
-      <c r="D5">
-        <v>35</v>
-      </c>
-      <c r="E5">
         <v>1835</v>
       </c>
     </row>
@@ -1450,7 +1433,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1514,7 +1497,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1578,7 +1561,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1634,7 +1617,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1642,7 +1625,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1659,35 +1642,52 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>244</v>
       </c>
       <c r="C2">
-        <v>1062</v>
+        <v>497</v>
       </c>
       <c r="D2">
-        <v>558</v>
+        <v>262</v>
       </c>
       <c r="E2">
-        <v>721</v>
+        <v>5067</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>1062</v>
+      </c>
+      <c r="D3">
+        <v>558</v>
+      </c>
+      <c r="E3">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>741</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>421</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>222</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>194</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Entropy Information Gain implemented in EDA to detect potentially important features
</commit_message>
<xml_diff>
--- a/Data-Analysis/CategoricalStats.xlsx
+++ b/Data-Analysis/CategoricalStats.xlsx
@@ -7,30 +7,88 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="sexo" sheetId="1" r:id="rId1"/>
-    <sheet name="dias_fiebre" sheetId="2" r:id="rId2"/>
-    <sheet name="dias_ultima_fiebre" sheetId="3" r:id="rId3"/>
-    <sheet name="nauseas" sheetId="4" r:id="rId4"/>
-    <sheet name="vomitos" sheetId="5" r:id="rId5"/>
-    <sheet name="rash" sheetId="6" r:id="rId6"/>
-    <sheet name="mialgias" sheetId="7" r:id="rId7"/>
-    <sheet name="artralgias" sheetId="8" r:id="rId8"/>
-    <sheet name="prueba_torniquete" sheetId="9" r:id="rId9"/>
-    <sheet name="dolor_abdominal" sheetId="10" r:id="rId10"/>
-    <sheet name="acumulacion_fluidos" sheetId="11" r:id="rId11"/>
-    <sheet name="sangrado_mucosas" sheetId="12" r:id="rId12"/>
-    <sheet name="hemorragia" sheetId="13" r:id="rId13"/>
-    <sheet name="shock" sheetId="14" r:id="rId14"/>
-    <sheet name="letargia" sheetId="15" r:id="rId15"/>
-    <sheet name="irritabilidad" sheetId="16" r:id="rId16"/>
-    <sheet name="hepatomegalia" sheetId="17" r:id="rId17"/>
+    <sheet name="Attribute" sheetId="1" r:id="rId1"/>
+    <sheet name="sexo" sheetId="2" r:id="rId2"/>
+    <sheet name="dias_fiebre" sheetId="3" r:id="rId3"/>
+    <sheet name="dias_ultima_fiebre" sheetId="4" r:id="rId4"/>
+    <sheet name="nauseas" sheetId="5" r:id="rId5"/>
+    <sheet name="vomitos" sheetId="6" r:id="rId6"/>
+    <sheet name="rash" sheetId="7" r:id="rId7"/>
+    <sheet name="mialgias" sheetId="8" r:id="rId8"/>
+    <sheet name="artralgias" sheetId="9" r:id="rId9"/>
+    <sheet name="prueba_torniquete" sheetId="10" r:id="rId10"/>
+    <sheet name="dolor_abdominal" sheetId="11" r:id="rId11"/>
+    <sheet name="acumulacion_fluidos" sheetId="12" r:id="rId12"/>
+    <sheet name="sangrado_mucosas" sheetId="13" r:id="rId13"/>
+    <sheet name="hemorragia" sheetId="14" r:id="rId14"/>
+    <sheet name="shock" sheetId="15" r:id="rId15"/>
+    <sheet name="letargia" sheetId="16" r:id="rId16"/>
+    <sheet name="irritabilidad" sheetId="17" r:id="rId17"/>
+    <sheet name="hepatomegalia" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="31">
+  <si>
+    <t>Information Gain</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>dias_fiebre</t>
+  </si>
+  <si>
+    <t>prueba_torniquete</t>
+  </si>
+  <si>
+    <t>sangrado_mucosas</t>
+  </si>
+  <si>
+    <t>vomitos</t>
+  </si>
+  <si>
+    <t>hepatomegalia</t>
+  </si>
+  <si>
+    <t>hemorragia</t>
+  </si>
+  <si>
+    <t>acumulacion_fluidos</t>
+  </si>
+  <si>
+    <t>letargia</t>
+  </si>
+  <si>
+    <t>artralgias</t>
+  </si>
+  <si>
+    <t>dias_ultima_fiebre</t>
+  </si>
+  <si>
+    <t>dolor_abdominal</t>
+  </si>
+  <si>
+    <t>rash</t>
+  </si>
+  <si>
+    <t>shock</t>
+  </si>
+  <si>
+    <t>nauseas</t>
+  </si>
+  <si>
+    <t>mialgias</t>
+  </si>
+  <si>
+    <t>irritabilidad</t>
+  </si>
+  <si>
+    <t>sexo</t>
+  </si>
   <si>
     <t>Dengue_Grave</t>
   </si>
@@ -44,48 +102,21 @@
     <t>No_Dengue</t>
   </si>
   <si>
-    <t>sexo</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>dias_fiebre</t>
-  </si>
-  <si>
-    <t>dias_ultima_fiebre</t>
-  </si>
-  <si>
-    <t>nauseas</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Si</t>
   </si>
   <si>
-    <t>vomitos</t>
-  </si>
-  <si>
     <t>Persistente</t>
   </si>
   <si>
-    <t>rash</t>
-  </si>
-  <si>
-    <t>mialgias</t>
-  </si>
-  <si>
-    <t>artralgias</t>
-  </si>
-  <si>
-    <t>prueba_torniquete</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -93,30 +124,6 @@
   </si>
   <si>
     <t>Positiva</t>
-  </si>
-  <si>
-    <t>dolor_abdominal</t>
-  </si>
-  <si>
-    <t>acumulacion_fluidos</t>
-  </si>
-  <si>
-    <t>sangrado_mucosas</t>
-  </si>
-  <si>
-    <t>hemorragia</t>
-  </si>
-  <si>
-    <t>shock</t>
-  </si>
-  <si>
-    <t>letargia</t>
-  </si>
-  <si>
-    <t>irritabilidad</t>
-  </si>
-  <si>
-    <t>hepatomegalia</t>
   </si>
 </sst>
 </file>
@@ -474,61 +481,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2">
+        <v>0.5099296808225293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="B3">
+        <v>0.3823835557956539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.2609249452030464</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>494</v>
-      </c>
-      <c r="C2">
-        <v>952</v>
-      </c>
-      <c r="D2">
-        <v>532</v>
-      </c>
-      <c r="E2">
-        <v>3068</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+      <c r="B5">
+        <v>0.236397074462362</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>502</v>
-      </c>
-      <c r="C3">
-        <v>1028</v>
-      </c>
-      <c r="D3">
-        <v>510</v>
-      </c>
-      <c r="E3">
-        <v>2914</v>
+      <c r="B6">
+        <v>0.2203654270545505</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.2189221877515564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.1959747016002418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.1730377090979678</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.115992925625698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0.1103135474878145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.09677906114456958</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.09575439241974193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.09330816329885039</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.03828545416201679</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.03431686224819885</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0.009816199409422799</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0.0004735832939239959</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +638,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -546,53 +646,70 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B2">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="C2">
-        <v>1799</v>
+        <v>497</v>
       </c>
       <c r="D2">
-        <v>671</v>
+        <v>262</v>
       </c>
       <c r="E2">
-        <v>3638</v>
+        <v>5067</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>723</v>
-      </c>
       <c r="C3">
-        <v>181</v>
+        <v>1062</v>
       </c>
       <c r="D3">
-        <v>371</v>
+        <v>558</v>
       </c>
       <c r="E3">
-        <v>2344</v>
+        <v>721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>741</v>
+      </c>
+      <c r="C4">
+        <v>421</v>
+      </c>
+      <c r="D4">
+        <v>222</v>
+      </c>
+      <c r="E4">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -610,53 +727,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="C2">
-        <v>1785</v>
+        <v>1799</v>
       </c>
       <c r="D2">
-        <v>658</v>
+        <v>671</v>
       </c>
       <c r="E2">
-        <v>5680</v>
+        <v>3638</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>745</v>
+        <v>723</v>
       </c>
       <c r="C3">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="D3">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="E3">
-        <v>302</v>
+        <v>2344</v>
       </c>
     </row>
   </sheetData>
@@ -674,53 +791,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>197</v>
+        <v>251</v>
       </c>
       <c r="C2">
-        <v>1867</v>
+        <v>1785</v>
       </c>
       <c r="D2">
-        <v>887</v>
+        <v>658</v>
       </c>
       <c r="E2">
-        <v>5918</v>
+        <v>5680</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>799</v>
+        <v>745</v>
       </c>
       <c r="C3">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="D3">
-        <v>155</v>
+        <v>384</v>
       </c>
       <c r="E3">
-        <v>64</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -738,53 +855,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>197</v>
       </c>
       <c r="C2">
-        <v>1980</v>
+        <v>1867</v>
       </c>
       <c r="D2">
-        <v>1042</v>
+        <v>887</v>
       </c>
       <c r="E2">
-        <v>4987</v>
+        <v>5918</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>799</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="E3">
-        <v>995</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -802,27 +919,27 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>592</v>
+        <v>197</v>
       </c>
       <c r="C2">
         <v>1980</v>
@@ -831,15 +948,15 @@
         <v>1042</v>
       </c>
       <c r="E2">
-        <v>5521</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>404</v>
+        <v>799</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -848,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>461</v>
+        <v>995</v>
       </c>
     </row>
   </sheetData>
@@ -866,53 +983,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>307</v>
+        <v>592</v>
       </c>
       <c r="C2">
-        <v>1797</v>
+        <v>1980</v>
       </c>
       <c r="D2">
-        <v>652</v>
+        <v>1042</v>
       </c>
       <c r="E2">
-        <v>5658</v>
+        <v>5521</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>689</v>
+        <v>404</v>
       </c>
       <c r="C3">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>390</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>324</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -930,53 +1047,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>923</v>
+        <v>307</v>
       </c>
       <c r="C2">
-        <v>1969</v>
+        <v>1797</v>
       </c>
       <c r="D2">
-        <v>1011</v>
+        <v>652</v>
       </c>
       <c r="E2">
-        <v>5682</v>
+        <v>5658</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>73</v>
+        <v>689</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>183</v>
       </c>
       <c r="D3">
-        <v>31</v>
+        <v>390</v>
       </c>
       <c r="E3">
-        <v>300</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -994,53 +1111,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>265</v>
+        <v>923</v>
       </c>
       <c r="C2">
-        <v>1832</v>
+        <v>1969</v>
       </c>
       <c r="D2">
-        <v>652</v>
+        <v>1011</v>
       </c>
       <c r="E2">
-        <v>5796</v>
+        <v>5682</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>73</v>
+      </c>
+      <c r="C3">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>731</v>
-      </c>
-      <c r="C3">
-        <v>148</v>
-      </c>
       <c r="D3">
-        <v>390</v>
+        <v>31</v>
       </c>
       <c r="E3">
-        <v>186</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1048,9 +1165,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1058,104 +1175,117 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1832</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>652</v>
       </c>
       <c r="E2">
-        <v>2419</v>
+        <v>5796</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>731</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="E3">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>324</v>
-      </c>
-      <c r="C4">
-        <v>1211</v>
-      </c>
-      <c r="D4">
-        <v>674</v>
-      </c>
-      <c r="E4">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>361</v>
-      </c>
-      <c r="C5">
-        <v>389</v>
-      </c>
-      <c r="D5">
-        <v>187</v>
-      </c>
-      <c r="E5">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>311</v>
-      </c>
-      <c r="C6">
-        <v>380</v>
-      </c>
-      <c r="D6">
-        <v>181</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>494</v>
+      </c>
+      <c r="C2">
+        <v>952</v>
+      </c>
+      <c r="D2">
+        <v>532</v>
+      </c>
+      <c r="E2">
+        <v>3068</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>502</v>
+      </c>
+      <c r="C3">
+        <v>1028</v>
+      </c>
+      <c r="D3">
+        <v>510</v>
+      </c>
+      <c r="E3">
+        <v>2914</v>
       </c>
     </row>
   </sheetData>
@@ -1173,19 +1303,134 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>324</v>
+      </c>
+      <c r="C4">
+        <v>1211</v>
+      </c>
+      <c r="D4">
+        <v>674</v>
+      </c>
+      <c r="E4">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>361</v>
+      </c>
+      <c r="C5">
+        <v>389</v>
+      </c>
+      <c r="D5">
+        <v>187</v>
+      </c>
+      <c r="E5">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>311</v>
+      </c>
+      <c r="C6">
+        <v>380</v>
+      </c>
+      <c r="D6">
+        <v>181</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1278,7 +1523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1288,24 +1533,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>386</v>
@@ -1322,7 +1567,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>610</v>
@@ -1342,7 +1587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1352,24 +1597,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>241</v>
@@ -1386,7 +1631,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>745</v>
@@ -1403,7 +1648,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -1416,70 +1661,6 @@
       </c>
       <c r="E4">
         <v>1835</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>531</v>
-      </c>
-      <c r="C2">
-        <v>1479</v>
-      </c>
-      <c r="D2">
-        <v>777</v>
-      </c>
-      <c r="E2">
-        <v>5659</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>465</v>
-      </c>
-      <c r="C3">
-        <v>501</v>
-      </c>
-      <c r="D3">
-        <v>265</v>
-      </c>
-      <c r="E3">
-        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -1497,53 +1678,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>178</v>
+        <v>531</v>
       </c>
       <c r="C2">
-        <v>395</v>
+        <v>1479</v>
       </c>
       <c r="D2">
-        <v>211</v>
+        <v>777</v>
       </c>
       <c r="E2">
-        <v>2378</v>
+        <v>5659</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>818</v>
+        <v>465</v>
       </c>
       <c r="C3">
-        <v>1585</v>
+        <v>501</v>
       </c>
       <c r="D3">
-        <v>831</v>
+        <v>265</v>
       </c>
       <c r="E3">
-        <v>3604</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -1564,50 +1745,50 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="C2">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D2">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="E2">
-        <v>3541</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>792</v>
+        <v>818</v>
       </c>
       <c r="C3">
-        <v>1583</v>
+        <v>1585</v>
       </c>
       <c r="D3">
-        <v>851</v>
+        <v>831</v>
       </c>
       <c r="E3">
-        <v>2441</v>
+        <v>3604</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1798,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1625,70 +1806,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>244</v>
+        <v>204</v>
       </c>
       <c r="C2">
-        <v>497</v>
+        <v>397</v>
       </c>
       <c r="D2">
-        <v>262</v>
+        <v>191</v>
       </c>
       <c r="E2">
-        <v>5067</v>
+        <v>3541</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>792</v>
       </c>
       <c r="C3">
-        <v>1062</v>
+        <v>1583</v>
       </c>
       <c r="D3">
-        <v>558</v>
+        <v>851</v>
       </c>
       <c r="E3">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>741</v>
-      </c>
-      <c r="C4">
-        <v>421</v>
-      </c>
-      <c r="D4">
-        <v>222</v>
-      </c>
-      <c r="E4">
-        <v>194</v>
+        <v>2441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>